<commit_message>
upgraded to version 1.11.2.2
</commit_message>
<xml_diff>
--- a/examples/vpcwebapp/xlsx/access.xlsx
+++ b/examples/vpcwebapp/xlsx/access.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/tabular-terraform/examples/vpcwebapp/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E1D638-5B78-0941-8165-5560A49F37FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE148527-615A-754E-B75F-0571BCF14750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="1820" windowWidth="30440" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="460" windowWidth="25600" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aclrules" sheetId="51" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="190">
   <si>
     <t>*name</t>
   </si>
@@ -184,12 +184,6 @@
     <t>*file</t>
   </si>
   <si>
-    <t>network-acls.tf</t>
-  </si>
-  <si>
-    <t>security-groups.tf</t>
-  </si>
-  <si>
     <t>"deny"</t>
   </si>
   <si>
@@ -427,9 +421,6 @@
     <t>tags</t>
   </si>
   <si>
-    <t>resource-groups.tf</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -602,6 +593,18 @@
   </si>
   <si>
     <t>network_id</t>
+  </si>
+  <si>
+    <t>main.tf</t>
+  </si>
+  <si>
+    <t>cis.tf</t>
+  </si>
+  <si>
+    <t>securitygroups.tf</t>
+  </si>
+  <si>
+    <t>networkacls.tf</t>
   </si>
 </sst>
 </file>
@@ -710,6 +713,66 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -781,66 +844,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1275,30 +1278,30 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{66B01468-17B1-DF49-BD45-B84826DE910D}" name="Table32" displayName="Table32" ref="A1:G4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{66B01468-17B1-DF49-BD45-B84826DE910D}" name="Table32" displayName="Table32" ref="A1:G4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:G4" xr:uid="{E53C9C86-FACA-2C40-85AF-B9BA3559B380}"/>
   <tableColumns count="7">
-    <tableColumn id="6" xr3:uid="{8F21586E-BECB-3F45-BEAA-A449A14BE047}" name="*file" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{4EF03EBF-5996-424F-93A5-4447C7F1B426}" name="*resource" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{C065294C-9139-324E-B19B-962D20BC4BE9}" name="*name" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{592C42FA-35FC-334C-9912-6BAE32344BD6}" name="*public_key" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{A36A827B-73DB-0749-B08B-5E9FBF4CF71C}" name="resource_group" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F6CE2A63-DCA4-AB46-AD6C-B729704A5EAC}" name="tags" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{461DC722-A60D-2D4E-8D06-0C3D76DA4F10}" name="comments" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{8F21586E-BECB-3F45-BEAA-A449A14BE047}" name="*file" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4EF03EBF-5996-424F-93A5-4447C7F1B426}" name="*resource" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{C065294C-9139-324E-B19B-962D20BC4BE9}" name="*name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{592C42FA-35FC-334C-9912-6BAE32344BD6}" name="*public_key" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A36A827B-73DB-0749-B08B-5E9FBF4CF71C}" name="resource_group" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F6CE2A63-DCA4-AB46-AD6C-B729704A5EAC}" name="tags" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{461DC722-A60D-2D4E-8D06-0C3D76DA4F10}" name="comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E8C732A8-0017-264D-8362-11409D4ADB8A}" name="Table329" displayName="Table329" ref="A1:E5" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E8C732A8-0017-264D-8362-11409D4ADB8A}" name="Table329" displayName="Table329" ref="A1:E5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E5" xr:uid="{853761A8-3C8D-D146-AF16-A9CD69B737CB}"/>
   <tableColumns count="5">
-    <tableColumn id="6" xr3:uid="{C7B59D49-52B4-E74B-980A-CBAA1960F9B9}" name="*file" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{0F8D8265-8F60-6746-958A-BB70EE098749}" name="*resource" dataDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{20125E38-3425-9540-8E50-F8247EA67681}" name="*name" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{50B39641-31D5-1A42-A833-F3F591AE4879}" name="tags" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{E9307884-D588-8840-BA44-7ABC5CDEF259}" name="comments" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{C7B59D49-52B4-E74B-980A-CBAA1960F9B9}" name="*file" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{0F8D8265-8F60-6746-958A-BB70EE098749}" name="*resource" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{20125E38-3425-9540-8E50-F8247EA67681}" name="*name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{50B39641-31D5-1A42-A833-F3F591AE4879}" name="tags" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E9307884-D588-8840-BA44-7ABC5CDEF259}" name="comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1419,32 +1422,32 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FBE293FA-80EC-F242-887C-B11422C1022D}" name="Table169" displayName="Table169" ref="A1:G5" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FBE293FA-80EC-F242-887C-B11422C1022D}" name="Table169" displayName="Table169" ref="A1:G5" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:G5" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="7">
-    <tableColumn id="5" xr3:uid="{1783CBE2-5818-4D4F-8A50-0D325E64887E}" name="*file" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{7D27F76A-C057-7B41-8211-3A3FA8658B48}" name="*resource" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{7E6DC40E-F6C9-C643-8520-0BEA365DF21F}" name="*name" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{F1EC0EF8-857C-F845-8233-1A4645A1D255}" name="*global" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{71D8A097-A059-D544-88DD-CC2EB82698A3}" name="location" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7C954070-A47C-BC40-B8B7-36A3A762A9FF}" name="resource_group" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{9825ACF3-765C-1A4C-8ED3-664BBDA75427}" name="comments" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{1783CBE2-5818-4D4F-8A50-0D325E64887E}" name="*file" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{7D27F76A-C057-7B41-8211-3A3FA8658B48}" name="*resource" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{7E6DC40E-F6C9-C643-8520-0BEA365DF21F}" name="*name" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{F1EC0EF8-857C-F845-8233-1A4645A1D255}" name="*global" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{71D8A097-A059-D544-88DD-CC2EB82698A3}" name="location" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{7C954070-A47C-BC40-B8B7-36A3A762A9FF}" name="resource_group" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{9825ACF3-765C-1A4C-8ED3-664BBDA75427}" name="comments" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7FF21D0D-5BB2-7147-81F3-634B6BBC66AE}" name="Table16910" displayName="Table16910" ref="A1:G5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7FF21D0D-5BB2-7147-81F3-634B6BBC66AE}" name="Table16910" displayName="Table16910" ref="A1:G5" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:G5" xr:uid="{6D379596-E186-C240-BBB4-B8E74F1D3D56}"/>
   <tableColumns count="7">
-    <tableColumn id="5" xr3:uid="{E861A381-AFF9-CC4F-88E6-39905BA5EA5A}" name="*file" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7EDBEE7E-8A29-A44F-B042-967D4F2FFCC7}" name="*resource" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{6F7F1276-5372-6340-899C-BF0D347BEE24}" name="name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1C7A2F6D-A0B2-C347-BF50-233D0B3D59D4}" name="*gateway" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{50AFBAF0-B636-BA4C-AB12-FA8E8220FEC3}" name="*network_type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{17DC867E-74AA-2A43-B864-99A770207616}" name="network_id" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{32EB9F06-C8B0-8440-BEC7-F21EB35097EC}" name="comments" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{E861A381-AFF9-CC4F-88E6-39905BA5EA5A}" name="*file" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{7EDBEE7E-8A29-A44F-B042-967D4F2FFCC7}" name="*resource" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{6F7F1276-5372-6340-899C-BF0D347BEE24}" name="name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{1C7A2F6D-A0B2-C347-BF50-233D0B3D59D4}" name="*gateway" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{50AFBAF0-B636-BA4C-AB12-FA8E8220FEC3}" name="*network_type" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{17DC867E-74AA-2A43-B864-99A770207616}" name="network_id" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{32EB9F06-C8B0-8440-BEC7-F21EB35097EC}" name="comments" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1766,54 +1769,54 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1830,28 +1833,28 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1869,21 +1872,21 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1921,19 +1924,19 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1950,28 +1953,28 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1993,21 +1996,21 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -2029,21 +2032,21 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -2065,21 +2068,21 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2097,12 +2100,12 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>17</v>
@@ -2111,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2129,21 +2132,21 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2165,21 +2168,21 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -2201,21 +2204,21 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -2253,19 +2256,19 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -2282,28 +2285,28 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
@@ -2325,21 +2328,21 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2361,21 +2364,21 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2397,21 +2400,21 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2429,12 +2432,12 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>17</v>
@@ -2443,7 +2446,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2461,21 +2464,21 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2497,21 +2500,21 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2549,19 +2552,19 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2578,28 +2581,28 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2617,21 +2620,21 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2726,37 +2729,37 @@
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2811,40 +2814,40 @@
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2902,89 +2905,89 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3021,9 +3024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D3370-44D8-0A42-8C42-E9D4E75B0DB2}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3063,45 +3064,45 @@
         <v>6</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3110,27 +3111,27 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3139,27 +3140,27 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3168,27 +3169,27 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3201,27 +3202,27 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -3234,27 +3235,27 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -3263,7 +3264,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3283,22 +3284,22 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -3307,27 +3308,27 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -3336,27 +3337,27 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -3365,27 +3366,27 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -3398,27 +3399,27 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -3431,27 +3432,27 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -3460,7 +3461,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3480,22 +3481,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -3508,27 +3509,27 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
@@ -3539,27 +3540,27 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -3572,7 +3573,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -3592,22 +3593,22 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -3620,27 +3621,27 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -3653,27 +3654,27 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -3686,27 +3687,27 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -3719,27 +3720,27 @@
         <v>53</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>41</v>
@@ -3756,7 +3757,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -3850,7 +3851,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -3953,7 +3954,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -4043,54 +4044,54 @@
         <v>0</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4167,72 +4168,72 @@
         <v>0</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4241,36 +4242,36 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -4279,7 +4280,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4400,16 +4401,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -4497,19 +4498,19 @@
         <v>16</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>188</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>